<commit_message>
more functions implemented on the xlsx tool
</commit_message>
<xml_diff>
--- a/tools/xlsxfiles/tmp.xlsx
+++ b/tools/xlsxfiles/tmp.xlsx
@@ -17,23 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
-    </font>
-    <font>
-      <color rgb="000000FF"/>
-    </font>
-    <font>
-      <color rgb="000000FF"/>
-      <u val="single"/>
     </font>
   </fonts>
   <fills count="2">
@@ -44,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -52,15 +42,71 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick"/>
+      <right style="thick"/>
+      <top style="thick"/>
+      <bottom style="thick"/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick"/>
+      <top style="thick"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick"/>
+      <right/>
+      <top/>
+      <bottom style="thick"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick"/>
+      <top/>
+      <bottom style="thick"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -426,7 +472,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:L18"/>
+  <dimension ref="B1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -435,116 +481,153 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>wassup</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" s="1" t="inlineStr">
-        <is>
-          <t>wassupddd</t>
-        </is>
-      </c>
+      <c r="B1" s="1" t="n"/>
+      <c r="C1" s="1" t="n"/>
+      <c r="D1" s="1" t="n"/>
+    </row>
+    <row r="2">
+      <c r="B2" s="1" t="n"/>
+      <c r="C2" s="1" t="n"/>
+      <c r="D2" s="1" t="n"/>
+    </row>
+    <row r="3">
+      <c r="B3" s="1" t="n"/>
+      <c r="C3" s="1" t="n"/>
+      <c r="D3" s="1" t="n"/>
     </row>
     <row r="6">
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>wassupddd</t>
+      <c r="F6" s="2" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="G6" s="2" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="H6" s="2" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="I6" s="2" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="J6" s="2" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="K6" s="2" t="inlineStr">
+        <is>
+          <t>f</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="C7" s="3" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
+      <c r="F7" s="1" t="n"/>
+      <c r="G7" s="1" t="n"/>
+      <c r="H7" s="1" t="n"/>
+      <c r="I7" s="1" t="n"/>
+      <c r="J7" s="1" t="n"/>
+      <c r="K7" s="1" t="n"/>
+    </row>
+    <row r="8">
+      <c r="F8" s="1" t="n"/>
+      <c r="G8" s="1" t="n"/>
+      <c r="H8" s="1" t="n"/>
+      <c r="I8" s="1" t="n"/>
+      <c r="J8" s="1" t="n"/>
+      <c r="K8" s="1" t="n"/>
+    </row>
+    <row r="9">
+      <c r="F9" s="1" t="n"/>
+      <c r="G9" s="1" t="n"/>
+      <c r="H9" s="1" t="n"/>
+      <c r="I9" s="2" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="J9" s="1" t="n"/>
+      <c r="K9" s="1" t="n"/>
+      <c r="L9" s="1" t="n"/>
+      <c r="M9" s="1" t="n"/>
+      <c r="N9" s="1" t="n"/>
     </row>
     <row r="10">
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
+      <c r="F10" s="1" t="n"/>
+      <c r="G10" s="1" t="n"/>
+      <c r="H10" s="1" t="n"/>
+      <c r="I10" s="2" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="J10" s="1" t="n"/>
+      <c r="K10" s="1" t="n"/>
+      <c r="L10" s="1" t="n"/>
+      <c r="M10" s="1" t="n"/>
+      <c r="N10" s="1" t="n"/>
+    </row>
+    <row r="11">
+      <c r="F11" s="1" t="n"/>
+      <c r="G11" s="1" t="n"/>
+      <c r="H11" s="1" t="n"/>
+      <c r="I11" s="2" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="J11" s="1" t="n"/>
+      <c r="K11" s="1" t="n"/>
+      <c r="L11" s="1" t="n"/>
+      <c r="M11" s="1" t="n"/>
+      <c r="N11" s="1" t="n"/>
     </row>
     <row r="12">
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
+      <c r="I12" s="2" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="J12" s="1" t="n"/>
+      <c r="K12" s="1" t="n"/>
+      <c r="L12" s="1" t="n"/>
+      <c r="M12" s="1" t="n"/>
+      <c r="N12" s="1" t="n"/>
+    </row>
+    <row r="13">
+      <c r="I13" s="2" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="J13" s="1" t="n"/>
+      <c r="K13" s="1" t="n"/>
+      <c r="L13" s="1" t="n"/>
+      <c r="M13" s="1" t="n"/>
+      <c r="N13" s="1" t="n"/>
     </row>
     <row r="14">
-      <c r="B14" s="1" t="inlineStr">
-        <is>
-          <t>wassupddd</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>blue red blue</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>hey bye</t>
-        </is>
-      </c>
+      <c r="I14" s="2" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="J14" s="1" t="n"/>
+      <c r="K14" s="1" t="n"/>
+      <c r="L14" s="1" t="n"/>
+      <c r="M14" s="1" t="n"/>
+      <c r="N14" s="1" t="n"/>
     </row>
   </sheetData>
-  <dataValidations count="14">
-    <dataValidation sqref="J10" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"A,B,C"</formula1>
-    </dataValidation>
-    <dataValidation sqref="J10" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"A,B,C"</formula1>
-    </dataValidation>
-    <dataValidation sqref="J10" showDropDown="1" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"A,B,C"</formula1>
-    </dataValidation>
-    <dataValidation sqref="J10" showDropDown="1" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"A,B,C"</formula1>
-    </dataValidation>
-    <dataValidation sqref="J10" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"A,B,C"</formula1>
-    </dataValidation>
-    <dataValidation sqref="J10" showDropDown="1" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"A,B,C"</formula1>
-    </dataValidation>
-    <dataValidation sqref="J10" showDropDown="1" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"A,B,C"</formula1>
-    </dataValidation>
-    <dataValidation sqref="J10" showDropDown="1" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"A,B,C"</formula1>
-    </dataValidation>
-    <dataValidation sqref="J10" showDropDown="1" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"A,B,C"</formula1>
-    </dataValidation>
-    <dataValidation sqref="L12" showDropDown="1" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"A,B,C"</formula1>
-    </dataValidation>
-    <dataValidation sqref="L12" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"A,B,C"</formula1>
-    </dataValidation>
-    <dataValidation sqref="L12" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
-      <formula1>"A,B,C"</formula1>
-    </dataValidation>
-    <dataValidation sqref="L12" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Please select a value from the dropdown list" type="list" errorStyle="stop">
-      <formula1>"A,B,C"</formula1>
-    </dataValidation>
-    <dataValidation sqref="L12" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Please select a value from the dropdown list" type="list" errorStyle="stop">
-      <formula1>"A,B,C"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C7" r:id="rId1"/>
-  </hyperlinks>
+  <mergeCells count="1">
+    <mergeCell ref="B1:D3"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
made all the diary tool basic features
</commit_message>
<xml_diff>
--- a/tools/xlsxfiles/tmp.xlsx
+++ b/tools/xlsxfiles/tmp.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -25,16 +25,38 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <color rgb="000000FF"/>
+      <u val="single"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFF00"/>
+        <bgColor rgb="00FFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00A199A8"/>
+        <bgColor rgb="00A199A8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="005FBCFA"/>
+        <bgColor rgb="005FBCFA"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -43,69 +65,38 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick"/>
-      <right style="thick"/>
-      <top style="thick"/>
-      <bottom style="thick"/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thick"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick"/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick"/>
-      <top style="thick"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick"/>
-      <right/>
-      <top/>
-      <bottom style="thick"/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick"/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick"/>
-      <top/>
-      <bottom style="thick"/>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -472,7 +463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:N14"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,154 +471,251 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="n"/>
-      <c r="C1" s="1" t="n"/>
-      <c r="D1" s="1" t="n"/>
+    <row r="1" ht="65" customHeight="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Intern Instructions: The work diary is meant to help you track your progress over the summer, reflect on your accomplishments, and support conversations with your manager, team buddy, or mentor. It will also serve as a 
+helpful reference when you complete a competency document later in your internship. Please remove examples below and fill in your own entries weekly, this should take no more than 15 minutes each week.</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="n"/>
+      <c r="C1" s="2" t="n"/>
+      <c r="D1" s="2" t="n"/>
+      <c r="E1" s="2" t="n"/>
+      <c r="F1" s="2" t="n"/>
+      <c r="G1" s="2" t="n"/>
+      <c r="H1" s="2" t="n"/>
+      <c r="I1" s="2" t="n"/>
+      <c r="J1" s="2" t="n"/>
+      <c r="K1" s="2" t="n"/>
+      <c r="L1" s="2" t="n"/>
+      <c r="M1" s="2" t="n"/>
+      <c r="N1" s="2" t="n"/>
+      <c r="O1" s="2" t="n"/>
+      <c r="P1" s="2" t="n"/>
+      <c r="Q1" s="2" t="n"/>
+      <c r="R1" s="2" t="n"/>
+      <c r="S1" s="2" t="n"/>
+      <c r="T1" s="2" t="n"/>
     </row>
-    <row r="2">
-      <c r="B2" s="1" t="n"/>
-      <c r="C2" s="1" t="n"/>
-      <c r="D2" s="1" t="n"/>
+    <row r="2" ht="40" customHeight="1">
+      <c r="A2" s="3" t="n"/>
+      <c r="B2" s="4" t="inlineStr">
+        <is>
+          <t>Ran Wurmbrand</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="n"/>
+      <c r="D2" s="3" t="n"/>
+      <c r="E2" s="3" t="n"/>
+      <c r="F2" s="3" t="n"/>
+      <c r="G2" s="3" t="n"/>
+      <c r="H2" s="3" t="n"/>
+      <c r="I2" s="4" t="inlineStr">
+        <is>
+          <t>Konveyor-AI</t>
+        </is>
+      </c>
+      <c r="J2" s="3" t="n"/>
+      <c r="K2" s="3" t="n"/>
+      <c r="L2" s="3" t="n"/>
+      <c r="M2" s="3" t="n"/>
+      <c r="N2" s="4" t="inlineStr">
+        <is>
+          <t>Ilanit Stein</t>
+        </is>
+      </c>
+      <c r="O2" s="3" t="n"/>
+      <c r="P2" s="3" t="n"/>
+      <c r="Q2" s="3" t="n"/>
+      <c r="R2" s="3" t="n"/>
+      <c r="S2" s="3" t="n"/>
+      <c r="T2" s="3" t="n"/>
     </row>
     <row r="3">
-      <c r="B3" s="1" t="n"/>
-      <c r="C3" s="1" t="n"/>
-      <c r="D3" s="1" t="n"/>
+      <c r="B3" s="5" t="inlineStr">
+        <is>
+          <t>Jira</t>
+        </is>
+      </c>
+      <c r="C3" s="6" t="inlineStr">
+        <is>
+          <t>jira</t>
+        </is>
+      </c>
+      <c r="D3" s="6" t="inlineStr">
+        <is>
+          <t>google</t>
+        </is>
+      </c>
     </row>
-    <row r="6">
-      <c r="F6" s="2" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="G6" s="2" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="H6" s="2" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="I6" s="2" t="inlineStr">
-        <is>
-          <t>d</t>
-        </is>
-      </c>
-      <c r="J6" s="2" t="inlineStr">
-        <is>
-          <t>e</t>
-        </is>
-      </c>
-      <c r="K6" s="2" t="inlineStr">
-        <is>
-          <t>f</t>
-        </is>
-      </c>
+    <row r="4">
+      <c r="B4" s="5" t="inlineStr">
+        <is>
+          <t>Github</t>
+        </is>
+      </c>
+      <c r="C4" s="6" t="inlineStr">
+        <is>
+          <t>github</t>
+        </is>
+      </c>
+      <c r="D4" s="7" t="n"/>
+    </row>
+    <row r="6" ht="25" customHeight="1">
+      <c r="A6" s="8" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B6" s="9" t="n"/>
+      <c r="C6" s="8" t="inlineStr">
+        <is>
+          <t>Effort Type</t>
+        </is>
+      </c>
+      <c r="D6" s="9" t="n"/>
+      <c r="E6" s="9" t="n"/>
+      <c r="F6" s="8" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="G6" s="9" t="n"/>
+      <c r="H6" s="9" t="n"/>
+      <c r="I6" s="8" t="inlineStr">
+        <is>
+          <t>Links</t>
+        </is>
+      </c>
+      <c r="J6" s="9" t="n"/>
+      <c r="K6" s="9" t="n"/>
+      <c r="L6" s="8" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="M6" s="9" t="n"/>
+      <c r="N6" s="9" t="n"/>
+      <c r="O6" s="8" t="inlineStr">
+        <is>
+          <t>Impact/OutCome</t>
+        </is>
+      </c>
+      <c r="P6" s="9" t="n"/>
+      <c r="Q6" s="9" t="n"/>
+      <c r="R6" s="8" t="inlineStr">
+        <is>
+          <t>Additional Notes</t>
+        </is>
+      </c>
+      <c r="S6" s="9" t="n"/>
+      <c r="T6" s="9" t="n"/>
     </row>
     <row r="7">
-      <c r="F7" s="1" t="n"/>
-      <c r="G7" s="1" t="n"/>
-      <c r="H7" s="1" t="n"/>
-      <c r="I7" s="1" t="n"/>
-      <c r="J7" s="1" t="n"/>
-      <c r="K7" s="1" t="n"/>
+      <c r="A7" s="4" t="inlineStr">
+        <is>
+          <t>week 1 (jun 8 - jun 14)</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="n"/>
+      <c r="C7" s="3" t="n"/>
+      <c r="D7" s="3" t="n"/>
+      <c r="E7" s="3" t="n"/>
+      <c r="F7" s="3" t="n"/>
+      <c r="G7" s="3" t="n"/>
+      <c r="H7" s="3" t="n"/>
+      <c r="I7" s="3" t="n"/>
+      <c r="J7" s="3" t="n"/>
+      <c r="K7" s="3" t="n"/>
+      <c r="L7" s="3" t="n"/>
+      <c r="M7" s="3" t="n"/>
+      <c r="N7" s="3" t="n"/>
+      <c r="O7" s="3" t="n"/>
+      <c r="P7" s="3" t="n"/>
+      <c r="Q7" s="3" t="n"/>
+      <c r="R7" s="3" t="n"/>
+      <c r="S7" s="3" t="n"/>
+      <c r="T7" s="3" t="n"/>
     </row>
     <row r="8">
-      <c r="F8" s="1" t="n"/>
-      <c r="G8" s="1" t="n"/>
-      <c r="H8" s="1" t="n"/>
-      <c r="I8" s="1" t="n"/>
-      <c r="J8" s="1" t="n"/>
-      <c r="K8" s="1" t="n"/>
-    </row>
-    <row r="9">
-      <c r="F9" s="1" t="n"/>
-      <c r="G9" s="1" t="n"/>
-      <c r="H9" s="1" t="n"/>
-      <c r="I9" s="2" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="J9" s="1" t="n"/>
-      <c r="K9" s="1" t="n"/>
-      <c r="L9" s="1" t="n"/>
-      <c r="M9" s="1" t="n"/>
-      <c r="N9" s="1" t="n"/>
-    </row>
-    <row r="10">
-      <c r="F10" s="1" t="n"/>
-      <c r="G10" s="1" t="n"/>
-      <c r="H10" s="1" t="n"/>
-      <c r="I10" s="2" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="J10" s="1" t="n"/>
-      <c r="K10" s="1" t="n"/>
-      <c r="L10" s="1" t="n"/>
-      <c r="M10" s="1" t="n"/>
-      <c r="N10" s="1" t="n"/>
-    </row>
-    <row r="11">
-      <c r="F11" s="1" t="n"/>
-      <c r="G11" s="1" t="n"/>
-      <c r="H11" s="1" t="n"/>
-      <c r="I11" s="2" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="J11" s="1" t="n"/>
-      <c r="K11" s="1" t="n"/>
-      <c r="L11" s="1" t="n"/>
-      <c r="M11" s="1" t="n"/>
-      <c r="N11" s="1" t="n"/>
-    </row>
-    <row r="12">
-      <c r="I12" s="2" t="inlineStr">
-        <is>
-          <t>d</t>
-        </is>
-      </c>
-      <c r="J12" s="1" t="n"/>
-      <c r="K12" s="1" t="n"/>
-      <c r="L12" s="1" t="n"/>
-      <c r="M12" s="1" t="n"/>
-      <c r="N12" s="1" t="n"/>
-    </row>
-    <row r="13">
-      <c r="I13" s="2" t="inlineStr">
-        <is>
-          <t>e</t>
-        </is>
-      </c>
-      <c r="J13" s="1" t="n"/>
-      <c r="K13" s="1" t="n"/>
-      <c r="L13" s="1" t="n"/>
-      <c r="M13" s="1" t="n"/>
-      <c r="N13" s="1" t="n"/>
-    </row>
-    <row r="14">
-      <c r="I14" s="2" t="inlineStr">
-        <is>
-          <t>f</t>
-        </is>
-      </c>
-      <c r="J14" s="1" t="n"/>
-      <c r="K14" s="1" t="n"/>
-      <c r="L14" s="1" t="n"/>
-      <c r="M14" s="1" t="n"/>
-      <c r="N14" s="1" t="n"/>
+      <c r="A8" s="10" t="inlineStr">
+        <is>
+          <t>jun 15</t>
+        </is>
+      </c>
+      <c r="B8" s="7" t="n"/>
+      <c r="C8" s="10" t="inlineStr">
+        <is>
+          <t>medium</t>
+        </is>
+      </c>
+      <c r="D8" s="7" t="n"/>
+      <c r="E8" s="7" t="n"/>
+      <c r="F8" s="10" t="inlineStr">
+        <is>
+          <t>reateing diary tool</t>
+        </is>
+      </c>
+      <c r="G8" s="7" t="n"/>
+      <c r="H8" s="7" t="n"/>
+      <c r="I8" s="6" t="inlineStr">
+        <is>
+          <t>google</t>
+        </is>
+      </c>
+      <c r="J8" s="7" t="n"/>
+      <c r="K8" s="7" t="n"/>
+      <c r="L8" s="10" t="inlineStr">
+        <is>
+          <t>in progras</t>
+        </is>
+      </c>
+      <c r="M8" s="7" t="n"/>
+      <c r="N8" s="7" t="n"/>
+      <c r="O8" s="10" t="inlineStr">
+        <is>
+          <t>make an inside tool at redhat</t>
+        </is>
+      </c>
+      <c r="P8" s="7" t="n"/>
+      <c r="Q8" s="7" t="n"/>
+      <c r="R8" s="10" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="S8" s="7" t="n"/>
+      <c r="T8" s="7" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:D3"/>
+  <mergeCells count="19">
+    <mergeCell ref="I2:M2"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="A7:T7"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="N2:T2"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="R6:T6"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C3" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D3" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C4" r:id="rId3"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I8" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>